<commit_message>
Updated from Python script
</commit_message>
<xml_diff>
--- a/data/level_1.xlsx
+++ b/data/level_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jzhu/Downloads/Bread/Loyalty/Loyalty_Control/data_/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jzhu/Downloads/Bread/Loyalty/Loyalty_Control/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7978F275-1AD5-3F4B-9A15-B1EB777B145D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8A0C28-0021-5A4A-9C27-96152A85A94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6340" yWindow="6040" windowWidth="27640" windowHeight="16940" xr2:uid="{AB0E122F-5828-C241-B840-7FB204FB6038}"/>
+    <workbookView xWindow="5960" yWindow="3180" windowWidth="27640" windowHeight="16940" xr2:uid="{AB0E122F-5828-C241-B840-7FB204FB6038}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>Client ID</t>
   </si>
   <si>
-    <t>Prin ID</t>
-  </si>
-  <si>
-    <t>Prin Description</t>
-  </si>
-  <si>
     <t>As of Date</t>
   </si>
   <si>
@@ -90,6 +84,12 @@
   </si>
   <si>
     <t>POINTS MASTERCARD</t>
+  </si>
+  <si>
+    <t>Partner ID</t>
+  </si>
+  <si>
+    <t>Partner Description</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,31 +561,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -596,7 +596,7 @@
         <v>502</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="6">
         <v>44987</v>
@@ -617,7 +617,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -628,7 +628,7 @@
         <v>517</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6">
         <v>44987</v>
@@ -649,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>466</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="6">
         <v>44987</v>
@@ -681,7 +681,7 @@
         <v>4</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -692,7 +692,7 @@
         <v>482</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6">
         <v>44987</v>
@@ -713,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -724,7 +724,7 @@
         <v>494</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="6">
         <v>44987</v>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -756,7 +756,7 @@
         <v>799</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="6">
         <v>44987</v>
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>